<commit_message>
Assign SKHU Value: 50%
</commit_message>
<xml_diff>
--- a/public/Dataset/Dataset UP.xlsx
+++ b/public/Dataset/Dataset UP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File\UNDIP\PKL\template excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imbecile\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F1C7AE-900B-4F6E-84B4-175F0DEF1C8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D58C90B-0240-4E1D-886A-D009637E97D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7DB892E0-464B-4B00-9D0F-F52A699E8CE8}"/>
   </bookViews>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30033CE3-F2BE-4385-9354-DFF71185792E}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,13 +512,13 @@
         <v>1001</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -527,33 +527,1783 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="P2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="1">
+        <v>80</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>69</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>64</v>
+      </c>
+      <c r="H3" s="1">
+        <v>79</v>
+      </c>
+      <c r="I3" s="1">
+        <v>57</v>
+      </c>
+      <c r="J3" s="1">
+        <v>92</v>
+      </c>
+      <c r="K3" s="1">
+        <v>79</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>82</v>
+      </c>
+      <c r="N3" s="1">
+        <v>97</v>
+      </c>
+      <c r="O3" s="1">
+        <v>78</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" s="1">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>95</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>92</v>
+      </c>
+      <c r="H4" s="1">
+        <v>99</v>
+      </c>
+      <c r="I4" s="1">
+        <v>97</v>
+      </c>
+      <c r="J4" s="1">
+        <v>78</v>
+      </c>
+      <c r="K4" s="1">
+        <v>61</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>95</v>
+      </c>
+      <c r="N4" s="1">
+        <v>79</v>
+      </c>
+      <c r="O4" s="1">
+        <v>58</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" s="1">
+        <v>79</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>91</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>61</v>
+      </c>
+      <c r="H5" s="1">
+        <v>64</v>
+      </c>
+      <c r="I5" s="1">
+        <v>74</v>
+      </c>
+      <c r="J5" s="1">
+        <v>89</v>
+      </c>
+      <c r="K5" s="1">
+        <v>91</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>87</v>
+      </c>
+      <c r="N5" s="1">
+        <v>100</v>
+      </c>
+      <c r="O5" s="1">
+        <v>50</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" s="1">
+        <v>83</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>87</v>
+      </c>
+      <c r="H6" s="1">
+        <v>81</v>
+      </c>
+      <c r="I6" s="1">
+        <v>94</v>
+      </c>
+      <c r="J6" s="1">
+        <v>70</v>
+      </c>
+      <c r="K6" s="1">
+        <v>60</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>90</v>
+      </c>
+      <c r="N6" s="1">
+        <v>84</v>
+      </c>
+      <c r="O6" s="1">
+        <v>59</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1006</v>
+      </c>
+      <c r="B7" s="1">
+        <v>97</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>95</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>84</v>
+      </c>
+      <c r="H7" s="1">
+        <v>84</v>
+      </c>
+      <c r="I7" s="1">
+        <v>63</v>
+      </c>
+      <c r="J7" s="1">
+        <v>79</v>
+      </c>
+      <c r="K7" s="1">
+        <v>96</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>80</v>
+      </c>
+      <c r="N7" s="1">
+        <v>70</v>
+      </c>
+      <c r="O7" s="1">
+        <v>84</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1007</v>
+      </c>
+      <c r="B8" s="1">
+        <v>96</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>98</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>69</v>
+      </c>
+      <c r="H8" s="1">
+        <v>76</v>
+      </c>
+      <c r="I8" s="1">
+        <v>66</v>
+      </c>
+      <c r="J8" s="1">
+        <v>96</v>
+      </c>
+      <c r="K8" s="1">
+        <v>98</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>80</v>
+      </c>
+      <c r="N8" s="1">
+        <v>87</v>
+      </c>
+      <c r="O8" s="1">
+        <v>55</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1008</v>
+      </c>
+      <c r="B9" s="1">
+        <v>93</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>82</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>98</v>
+      </c>
+      <c r="H9" s="1">
+        <v>64</v>
+      </c>
+      <c r="I9" s="1">
+        <v>89</v>
+      </c>
+      <c r="J9" s="1">
+        <v>77</v>
+      </c>
+      <c r="K9" s="1">
+        <v>86</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>89</v>
+      </c>
+      <c r="N9" s="1">
+        <v>94</v>
+      </c>
+      <c r="O9" s="1">
+        <v>94</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1009</v>
+      </c>
+      <c r="B10" s="1">
+        <v>79</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>69</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>79</v>
+      </c>
+      <c r="H10" s="1">
+        <v>96</v>
+      </c>
+      <c r="I10" s="1">
+        <v>83</v>
+      </c>
+      <c r="J10" s="1">
+        <v>92</v>
+      </c>
+      <c r="K10" s="1">
+        <v>97</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>94</v>
+      </c>
+      <c r="N10" s="1">
+        <v>70</v>
+      </c>
+      <c r="O10" s="1">
+        <v>99</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1010</v>
+      </c>
+      <c r="B11" s="1">
+        <v>71</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>83</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>71</v>
+      </c>
+      <c r="H11" s="1">
+        <v>100</v>
+      </c>
+      <c r="I11" s="1">
+        <v>84</v>
+      </c>
+      <c r="J11" s="1">
+        <v>71</v>
+      </c>
+      <c r="K11" s="1">
+        <v>68</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>84</v>
+      </c>
+      <c r="N11" s="1">
+        <v>91</v>
+      </c>
+      <c r="O11" s="1">
+        <v>81</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1011</v>
+      </c>
+      <c r="B12" s="1">
+        <v>89</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>87</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>69</v>
+      </c>
+      <c r="H12" s="1">
+        <v>88</v>
+      </c>
+      <c r="I12" s="1">
+        <v>98</v>
+      </c>
+      <c r="J12" s="1">
+        <v>73</v>
+      </c>
+      <c r="K12" s="1">
+        <v>86</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>91</v>
+      </c>
+      <c r="N12" s="1">
+        <v>91</v>
+      </c>
+      <c r="O12" s="1">
+        <v>58</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1012</v>
+      </c>
+      <c r="B13" s="1">
+        <v>72</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>98</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>68</v>
+      </c>
+      <c r="H13" s="1">
+        <v>68</v>
+      </c>
+      <c r="I13" s="1">
+        <v>87</v>
+      </c>
+      <c r="J13" s="1">
+        <v>78</v>
+      </c>
+      <c r="K13" s="1">
+        <v>93</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>89</v>
+      </c>
+      <c r="N13" s="1">
+        <v>91</v>
+      </c>
+      <c r="O13" s="1">
+        <v>64</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1013</v>
+      </c>
+      <c r="B14" s="1">
+        <v>90</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>65</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>93</v>
+      </c>
+      <c r="H14" s="1">
+        <v>65</v>
+      </c>
+      <c r="I14" s="1">
+        <v>83</v>
+      </c>
+      <c r="J14" s="1">
+        <v>73</v>
+      </c>
+      <c r="K14" s="1">
+        <v>87</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>81</v>
+      </c>
+      <c r="N14" s="1">
+        <v>91</v>
+      </c>
+      <c r="O14" s="1">
+        <v>66</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1014</v>
+      </c>
+      <c r="B15" s="1">
+        <v>92</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>67</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>62</v>
+      </c>
+      <c r="H15" s="1">
+        <v>100</v>
+      </c>
+      <c r="I15" s="1">
+        <v>66</v>
+      </c>
+      <c r="J15" s="1">
+        <v>87</v>
+      </c>
+      <c r="K15" s="1">
+        <v>88</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>88</v>
+      </c>
+      <c r="N15" s="1">
+        <v>85</v>
+      </c>
+      <c r="O15" s="1">
+        <v>59</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1015</v>
+      </c>
+      <c r="B16" s="1">
+        <v>85</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>90</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>87</v>
+      </c>
+      <c r="H16" s="1">
+        <v>94</v>
+      </c>
+      <c r="I16" s="1">
+        <v>80</v>
+      </c>
+      <c r="J16" s="1">
+        <v>82</v>
+      </c>
+      <c r="K16" s="1">
+        <v>78</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>88</v>
+      </c>
+      <c r="N16" s="1">
+        <v>84</v>
+      </c>
+      <c r="O16" s="1">
+        <v>93</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1016</v>
+      </c>
+      <c r="B17" s="1">
+        <v>77</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>69</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>95</v>
+      </c>
+      <c r="H17" s="1">
+        <v>96</v>
+      </c>
+      <c r="I17" s="1">
+        <v>58</v>
+      </c>
+      <c r="J17" s="1">
+        <v>92</v>
+      </c>
+      <c r="K17" s="1">
+        <v>60</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>82</v>
+      </c>
+      <c r="N17" s="1">
+        <v>77</v>
+      </c>
+      <c r="O17" s="1">
+        <v>98</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1017</v>
+      </c>
+      <c r="B18" s="1">
+        <v>72</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>100</v>
+      </c>
+      <c r="H18" s="1">
+        <v>64</v>
+      </c>
+      <c r="I18" s="1">
+        <v>55</v>
+      </c>
+      <c r="J18" s="1">
+        <v>83</v>
+      </c>
+      <c r="K18" s="1">
+        <v>60</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>86</v>
+      </c>
+      <c r="N18" s="1">
+        <v>98</v>
+      </c>
+      <c r="O18" s="1">
+        <v>72</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1018</v>
+      </c>
+      <c r="B19" s="1">
+        <v>94</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>98</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>92</v>
+      </c>
+      <c r="H19" s="1">
+        <v>94</v>
+      </c>
+      <c r="I19" s="1">
+        <v>86</v>
+      </c>
+      <c r="J19" s="1">
+        <v>75</v>
+      </c>
+      <c r="K19" s="1">
+        <v>79</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>94</v>
+      </c>
+      <c r="N19" s="1">
+        <v>77</v>
+      </c>
+      <c r="O19" s="1">
+        <v>57</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1019</v>
+      </c>
+      <c r="B20" s="1">
+        <v>99</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>64</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>88</v>
+      </c>
+      <c r="H20" s="1">
+        <v>80</v>
+      </c>
+      <c r="I20" s="1">
+        <v>79</v>
+      </c>
+      <c r="J20" s="1">
+        <v>73</v>
+      </c>
+      <c r="K20" s="1">
+        <v>78</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>97</v>
+      </c>
+      <c r="N20" s="1">
+        <v>82</v>
+      </c>
+      <c r="O20" s="1">
+        <v>50</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1020</v>
+      </c>
+      <c r="B21" s="1">
+        <v>81</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>89</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>75</v>
+      </c>
+      <c r="H21" s="1">
+        <v>91</v>
+      </c>
+      <c r="I21" s="1">
+        <v>51</v>
+      </c>
+      <c r="J21" s="1">
+        <v>90</v>
+      </c>
+      <c r="K21" s="1">
+        <v>100</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>97</v>
+      </c>
+      <c r="N21" s="1">
+        <v>82</v>
+      </c>
+      <c r="O21" s="1">
+        <v>100</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1021</v>
+      </c>
+      <c r="B22" s="1">
+        <v>90</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>76</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>83</v>
+      </c>
+      <c r="H22" s="1">
+        <v>94</v>
+      </c>
+      <c r="I22" s="1">
+        <v>75</v>
+      </c>
+      <c r="J22" s="1">
+        <v>89</v>
+      </c>
+      <c r="K22" s="1">
+        <v>76</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>84</v>
+      </c>
+      <c r="N22" s="1">
+        <v>97</v>
+      </c>
+      <c r="O22" s="1">
+        <v>66</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1022</v>
+      </c>
+      <c r="B23" s="1">
+        <v>94</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>67</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>100</v>
+      </c>
+      <c r="H23" s="1">
+        <v>100</v>
+      </c>
+      <c r="I23" s="1">
+        <v>78</v>
+      </c>
+      <c r="J23" s="1">
+        <v>77</v>
+      </c>
+      <c r="K23" s="1">
+        <v>95</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>98</v>
+      </c>
+      <c r="N23" s="1">
+        <v>79</v>
+      </c>
+      <c r="O23" s="1">
+        <v>75</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1023</v>
+      </c>
+      <c r="B24" s="1">
+        <v>90</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>62</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>93</v>
+      </c>
+      <c r="H24" s="1">
+        <v>70</v>
+      </c>
+      <c r="I24" s="1">
+        <v>93</v>
+      </c>
+      <c r="J24" s="1">
+        <v>73</v>
+      </c>
+      <c r="K24" s="1">
+        <v>73</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>84</v>
+      </c>
+      <c r="N24" s="1">
+        <v>87</v>
+      </c>
+      <c r="O24" s="1">
+        <v>86</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1024</v>
+      </c>
+      <c r="B25" s="1">
+        <v>81</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>96</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>100</v>
+      </c>
+      <c r="H25" s="1">
+        <v>86</v>
+      </c>
+      <c r="I25" s="1">
+        <v>51</v>
+      </c>
+      <c r="J25" s="1">
+        <v>91</v>
+      </c>
+      <c r="K25" s="1">
+        <v>91</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <v>95</v>
+      </c>
+      <c r="N25" s="1">
+        <v>75</v>
+      </c>
+      <c r="O25" s="1">
+        <v>66</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1025</v>
+      </c>
+      <c r="B26" s="1">
+        <v>75</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>71</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>88</v>
+      </c>
+      <c r="H26" s="1">
+        <v>97</v>
+      </c>
+      <c r="I26" s="1">
+        <v>51</v>
+      </c>
+      <c r="J26" s="1">
+        <v>90</v>
+      </c>
+      <c r="K26" s="1">
+        <v>85</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>80</v>
+      </c>
+      <c r="N26" s="1">
+        <v>89</v>
+      </c>
+      <c r="O26" s="1">
+        <v>66</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1026</v>
+      </c>
+      <c r="B27" s="1">
+        <v>79</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>95</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>61</v>
+      </c>
+      <c r="H27" s="1">
+        <v>97</v>
+      </c>
+      <c r="I27" s="1">
+        <v>57</v>
+      </c>
+      <c r="J27" s="1">
+        <v>79</v>
+      </c>
+      <c r="K27" s="1">
+        <v>92</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <v>100</v>
+      </c>
+      <c r="N27" s="1">
+        <v>89</v>
+      </c>
+      <c r="O27" s="1">
+        <v>96</v>
+      </c>
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1027</v>
+      </c>
+      <c r="B28" s="1">
+        <v>98</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>61</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>76</v>
+      </c>
+      <c r="H28" s="1">
+        <v>94</v>
+      </c>
+      <c r="I28" s="1">
+        <v>82</v>
+      </c>
+      <c r="J28" s="1">
+        <v>94</v>
+      </c>
+      <c r="K28" s="1">
+        <v>99</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
+        <v>93</v>
+      </c>
+      <c r="N28" s="1">
+        <v>87</v>
+      </c>
+      <c r="O28" s="1">
+        <v>98</v>
+      </c>
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1028</v>
+      </c>
+      <c r="B29" s="1">
+        <v>90</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>76</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>82</v>
+      </c>
+      <c r="H29" s="1">
+        <v>95</v>
+      </c>
+      <c r="I29" s="1">
+        <v>90</v>
+      </c>
+      <c r="J29" s="1">
+        <v>94</v>
+      </c>
+      <c r="K29" s="1">
+        <v>75</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>94</v>
+      </c>
+      <c r="N29" s="1">
+        <v>79</v>
+      </c>
+      <c r="O29" s="1">
+        <v>79</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1029</v>
+      </c>
+      <c r="B30" s="1">
+        <v>96</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>88</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>68</v>
+      </c>
+      <c r="H30" s="1">
+        <v>67</v>
+      </c>
+      <c r="I30" s="1">
+        <v>69</v>
+      </c>
+      <c r="J30" s="1">
+        <v>91</v>
+      </c>
+      <c r="K30" s="1">
+        <v>66</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>84</v>
+      </c>
+      <c r="N30" s="1">
+        <v>92</v>
+      </c>
+      <c r="O30" s="1">
+        <v>76</v>
+      </c>
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1030</v>
+      </c>
+      <c r="B31" s="1">
+        <v>90</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>76</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>61</v>
+      </c>
+      <c r="H31" s="1">
+        <v>93</v>
+      </c>
+      <c r="I31" s="1">
+        <v>85</v>
+      </c>
+      <c r="J31" s="1">
+        <v>89</v>
+      </c>
+      <c r="K31" s="1">
+        <v>84</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>95</v>
+      </c>
+      <c r="N31" s="1">
+        <v>83</v>
+      </c>
+      <c r="O31" s="1">
+        <v>100</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1031</v>
+      </c>
+      <c r="B32" s="1">
+        <v>71</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>98</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>72</v>
+      </c>
+      <c r="H32" s="1">
+        <v>73</v>
+      </c>
+      <c r="I32" s="1">
+        <v>90</v>
+      </c>
+      <c r="J32" s="1">
+        <v>88</v>
+      </c>
+      <c r="K32" s="1">
+        <v>80</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>88</v>
+      </c>
+      <c r="N32" s="1">
+        <v>83</v>
+      </c>
+      <c r="O32" s="1">
+        <v>51</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1032</v>
+      </c>
+      <c r="B33" s="1">
+        <v>83</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>67</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>98</v>
+      </c>
+      <c r="H33" s="1">
+        <v>65</v>
+      </c>
+      <c r="I33" s="1">
+        <v>70</v>
+      </c>
+      <c r="J33" s="1">
+        <v>82</v>
+      </c>
+      <c r="K33" s="1">
+        <v>74</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>92</v>
+      </c>
+      <c r="N33" s="1">
+        <v>98</v>
+      </c>
+      <c r="O33" s="1">
+        <v>96</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1033</v>
+      </c>
+      <c r="B34" s="1">
+        <v>87</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>64</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>61</v>
+      </c>
+      <c r="H34" s="1">
+        <v>76</v>
+      </c>
+      <c r="I34" s="1">
+        <v>98</v>
+      </c>
+      <c r="J34" s="1">
+        <v>74</v>
+      </c>
+      <c r="K34" s="1">
+        <v>80</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>85</v>
+      </c>
+      <c r="N34" s="1">
+        <v>92</v>
+      </c>
+      <c r="O34" s="1">
+        <v>97</v>
+      </c>
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1034</v>
+      </c>
+      <c r="B35" s="1">
+        <v>84</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>60</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>64</v>
+      </c>
+      <c r="H35" s="1">
+        <v>89</v>
+      </c>
+      <c r="I35" s="1">
+        <v>81</v>
+      </c>
+      <c r="J35" s="1">
+        <v>75</v>
+      </c>
+      <c r="K35" s="1">
+        <v>97</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>82</v>
+      </c>
+      <c r="N35" s="1">
+        <v>84</v>
+      </c>
+      <c r="O35" s="1">
+        <v>69</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1035</v>
+      </c>
+      <c r="B36" s="1">
+        <v>85</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>73</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>98</v>
+      </c>
+      <c r="H36" s="1">
+        <v>82</v>
+      </c>
+      <c r="I36" s="1">
+        <v>76</v>
+      </c>
+      <c r="J36" s="1">
+        <v>82</v>
+      </c>
+      <c r="K36" s="1">
+        <v>98</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>99</v>
+      </c>
+      <c r="N36" s="1">
+        <v>94</v>
+      </c>
+      <c r="O36" s="1">
+        <v>74</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1036</v>
+      </c>
+      <c r="B37" s="1">
+        <v>81</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>94</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>88</v>
+      </c>
+      <c r="H37" s="1">
+        <v>96</v>
+      </c>
+      <c r="I37" s="1">
+        <v>96</v>
+      </c>
+      <c r="J37" s="1">
+        <v>84</v>
+      </c>
+      <c r="K37" s="1">
+        <v>95</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>80</v>
+      </c>
+      <c r="N37" s="1">
+        <v>78</v>
+      </c>
+      <c r="O37" s="1">
+        <v>90</v>
+      </c>
+      <c r="P37" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assign final marks to SKHU
</commit_message>
<xml_diff>
--- a/public/Dataset/Dataset UP.xlsx
+++ b/public/Dataset/Dataset UP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imbecile\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File\UNDIP\PKL\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D58C90B-0240-4E1D-886A-D009637E97D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2950F2B2-87A3-41FD-9BF1-0F31C2696682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7DB892E0-464B-4B00-9D0F-F52A699E8CE8}"/>
   </bookViews>
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30033CE3-F2BE-4385-9354-DFF71185792E}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P37"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,49 +509,49 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1001</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1">
+        <v>87</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>82</v>
+      </c>
+      <c r="H2" s="1">
+        <v>90</v>
+      </c>
+      <c r="I2" s="1">
         <v>85</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>81</v>
-      </c>
-      <c r="H2" s="1">
-        <v>61</v>
-      </c>
-      <c r="I2" s="1">
-        <v>99</v>
-      </c>
       <c r="J2" s="1">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="K2" s="1">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
       </c>
       <c r="M2" s="1">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="N2" s="1">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="O2" s="1">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -559,16 +559,16 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1002</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -577,31 +577,31 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="H3" s="1">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="I3" s="1">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="J3" s="1">
+        <v>75</v>
+      </c>
+      <c r="K3" s="1">
         <v>92</v>
       </c>
-      <c r="K3" s="1">
-        <v>79</v>
-      </c>
       <c r="L3" s="1">
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="N3" s="1">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="O3" s="1">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
@@ -609,17 +609,17 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1003</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
         <v>100</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>95</v>
-      </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
@@ -627,31 +627,31 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H4" s="1">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="I4" s="1">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="J4" s="1">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="K4" s="1">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="L4" s="1">
         <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="N4" s="1">
         <v>79</v>
       </c>
       <c r="O4" s="1">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
@@ -659,16 +659,16 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1004</v>
+        <v>104</v>
       </c>
       <c r="B5" s="1">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -677,31 +677,31 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="H5" s="1">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I5" s="1">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J5" s="1">
         <v>89</v>
       </c>
       <c r="K5" s="1">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="N5" s="1">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="O5" s="1">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
@@ -709,16 +709,16 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1005</v>
+        <v>105</v>
       </c>
       <c r="B6" s="1">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -727,31 +727,31 @@
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H6" s="1">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="I6" s="1">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="J6" s="1">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K6" s="1">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="L6" s="1">
         <v>0</v>
       </c>
       <c r="M6" s="1">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="N6" s="1">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="O6" s="1">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="P6" s="1">
         <v>0</v>
@@ -759,16 +759,16 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1006</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -777,19 +777,19 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H7" s="1">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="I7" s="1">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="J7" s="1">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="K7" s="1">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
@@ -798,10 +798,10 @@
         <v>80</v>
       </c>
       <c r="N7" s="1">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O7" s="1">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
@@ -809,16 +809,16 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1007</v>
+        <v>107</v>
       </c>
       <c r="B8" s="1">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -827,31 +827,31 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H8" s="1">
+        <v>75</v>
+      </c>
+      <c r="I8" s="1">
+        <v>77</v>
+      </c>
+      <c r="J8" s="1">
+        <v>91</v>
+      </c>
+      <c r="K8" s="1">
+        <v>80</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <v>76</v>
       </c>
-      <c r="I8" s="1">
-        <v>66</v>
-      </c>
-      <c r="J8" s="1">
-        <v>96</v>
-      </c>
-      <c r="K8" s="1">
-        <v>98</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>80</v>
-      </c>
       <c r="N8" s="1">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="O8" s="1">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
@@ -859,16 +859,16 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1008</v>
+        <v>108</v>
       </c>
       <c r="B9" s="1">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -877,31 +877,31 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="H9" s="1">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="I9" s="1">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J9" s="1">
         <v>77</v>
       </c>
       <c r="K9" s="1">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="L9" s="1">
         <v>0</v>
       </c>
       <c r="M9" s="1">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="N9" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O9" s="1">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="P9" s="1">
         <v>0</v>
@@ -909,49 +909,49 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1009</v>
+        <v>109</v>
       </c>
       <c r="B10" s="1">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" s="1">
+        <v>90</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>88</v>
+      </c>
+      <c r="H10" s="1">
+        <v>97</v>
+      </c>
+      <c r="I10" s="1">
+        <v>72</v>
+      </c>
+      <c r="J10" s="1">
+        <v>90</v>
+      </c>
+      <c r="K10" s="1">
+        <v>87</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>75</v>
+      </c>
+      <c r="N10" s="1">
         <v>69</v>
       </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>79</v>
-      </c>
-      <c r="H10" s="1">
-        <v>96</v>
-      </c>
-      <c r="I10" s="1">
-        <v>83</v>
-      </c>
-      <c r="J10" s="1">
-        <v>92</v>
-      </c>
-      <c r="K10" s="1">
-        <v>97</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1">
-        <v>94</v>
-      </c>
-      <c r="N10" s="1">
-        <v>70</v>
-      </c>
       <c r="O10" s="1">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="P10" s="1">
         <v>0</v>
@@ -959,49 +959,49 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1010</v>
+        <v>110</v>
       </c>
       <c r="B11" s="1">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
       <c r="D11" s="1">
+        <v>91</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>78</v>
+      </c>
+      <c r="H11" s="1">
+        <v>81</v>
+      </c>
+      <c r="I11" s="1">
         <v>83</v>
       </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>71</v>
-      </c>
-      <c r="H11" s="1">
-        <v>100</v>
-      </c>
-      <c r="I11" s="1">
-        <v>84</v>
-      </c>
       <c r="J11" s="1">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="K11" s="1">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="L11" s="1">
         <v>0</v>
       </c>
       <c r="M11" s="1">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="N11" s="1">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="O11" s="1">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="P11" s="1">
         <v>0</v>
@@ -1009,49 +1009,49 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1011</v>
+        <v>111</v>
       </c>
       <c r="B12" s="1">
+        <v>62</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>88</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>88</v>
+      </c>
+      <c r="H12" s="1">
         <v>89</v>
       </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>87</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>69</v>
-      </c>
-      <c r="H12" s="1">
-        <v>88</v>
-      </c>
       <c r="I12" s="1">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="J12" s="1">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="K12" s="1">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12" s="1">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="N12" s="1">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="O12" s="1">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
@@ -1059,16 +1059,16 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1012</v>
+        <v>112</v>
       </c>
       <c r="B13" s="1">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -1077,31 +1077,31 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H13" s="1">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="I13" s="1">
+        <v>80</v>
+      </c>
+      <c r="J13" s="1">
+        <v>67</v>
+      </c>
+      <c r="K13" s="1">
+        <v>91</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>70</v>
+      </c>
+      <c r="N13" s="1">
         <v>87</v>
       </c>
-      <c r="J13" s="1">
-        <v>78</v>
-      </c>
-      <c r="K13" s="1">
-        <v>93</v>
-      </c>
-      <c r="L13" s="1">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1">
+      <c r="O13" s="1">
         <v>89</v>
-      </c>
-      <c r="N13" s="1">
-        <v>91</v>
-      </c>
-      <c r="O13" s="1">
-        <v>64</v>
       </c>
       <c r="P13" s="1">
         <v>0</v>
@@ -1109,16 +1109,16 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1013</v>
+        <v>113</v>
       </c>
       <c r="B14" s="1">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -1127,31 +1127,31 @@
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H14" s="1">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="I14" s="1">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J14" s="1">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="K14" s="1">
+        <v>84</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
         <v>87</v>
       </c>
-      <c r="L14" s="1">
-        <v>0</v>
-      </c>
-      <c r="M14" s="1">
-        <v>81</v>
-      </c>
       <c r="N14" s="1">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="O14" s="1">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="P14" s="1">
         <v>0</v>
@@ -1159,16 +1159,16 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1014</v>
+        <v>114</v>
       </c>
       <c r="B15" s="1">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1177,31 +1177,31 @@
         <v>0</v>
       </c>
       <c r="G15" s="1">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H15" s="1">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="I15" s="1">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="J15" s="1">
+        <v>50</v>
+      </c>
+      <c r="K15" s="1">
         <v>87</v>
       </c>
-      <c r="K15" s="1">
-        <v>88</v>
-      </c>
       <c r="L15" s="1">
         <v>0</v>
       </c>
       <c r="M15" s="1">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="N15" s="1">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="O15" s="1">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
@@ -1209,16 +1209,16 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1015</v>
+        <v>115</v>
       </c>
       <c r="B16" s="1">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -1227,31 +1227,31 @@
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="H16" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I16" s="1">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J16" s="1">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="K16" s="1">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="L16" s="1">
         <v>0</v>
       </c>
       <c r="M16" s="1">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="N16" s="1">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O16" s="1">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="P16" s="1">
         <v>0</v>
@@ -1259,16 +1259,16 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1016</v>
+        <v>116</v>
       </c>
       <c r="B17" s="1">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" s="1">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -1277,31 +1277,31 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
+        <v>75</v>
+      </c>
+      <c r="H17" s="1">
         <v>95</v>
       </c>
-      <c r="H17" s="1">
-        <v>96</v>
-      </c>
       <c r="I17" s="1">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="J17" s="1">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K17" s="1">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="L17" s="1">
         <v>0</v>
       </c>
       <c r="M17" s="1">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="N17" s="1">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="O17" s="1">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="P17" s="1">
         <v>0</v>
@@ -1309,16 +1309,16 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1017</v>
+        <v>117</v>
       </c>
       <c r="B18" s="1">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18" s="1">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -1327,31 +1327,31 @@
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H18" s="1">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="I18" s="1">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="J18" s="1">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="K18" s="1">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
       </c>
       <c r="M18" s="1">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="N18" s="1">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="O18" s="1">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="P18" s="1">
         <v>0</v>
@@ -1359,37 +1359,37 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1018</v>
+        <v>118</v>
       </c>
       <c r="B19" s="1">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" s="1">
+        <v>75</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>75</v>
+      </c>
+      <c r="H19" s="1">
+        <v>73</v>
+      </c>
+      <c r="I19" s="1">
+        <v>88</v>
+      </c>
+      <c r="J19" s="1">
+        <v>51</v>
+      </c>
+      <c r="K19" s="1">
         <v>98</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <v>92</v>
-      </c>
-      <c r="H19" s="1">
-        <v>94</v>
-      </c>
-      <c r="I19" s="1">
-        <v>86</v>
-      </c>
-      <c r="J19" s="1">
-        <v>75</v>
-      </c>
-      <c r="K19" s="1">
-        <v>79</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
@@ -1398,10 +1398,10 @@
         <v>94</v>
       </c>
       <c r="N19" s="1">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="O19" s="1">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
@@ -1409,16 +1409,16 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1019</v>
+        <v>119</v>
       </c>
       <c r="B20" s="1">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -1427,31 +1427,31 @@
         <v>0</v>
       </c>
       <c r="G20" s="1">
+        <v>81</v>
+      </c>
+      <c r="H20" s="1">
+        <v>85</v>
+      </c>
+      <c r="I20" s="1">
+        <v>71</v>
+      </c>
+      <c r="J20" s="1">
+        <v>94</v>
+      </c>
+      <c r="K20" s="1">
+        <v>92</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>89</v>
+      </c>
+      <c r="N20" s="1">
         <v>88</v>
       </c>
-      <c r="H20" s="1">
-        <v>80</v>
-      </c>
-      <c r="I20" s="1">
-        <v>79</v>
-      </c>
-      <c r="J20" s="1">
-        <v>73</v>
-      </c>
-      <c r="K20" s="1">
-        <v>78</v>
-      </c>
-      <c r="L20" s="1">
-        <v>0</v>
-      </c>
-      <c r="M20" s="1">
-        <v>97</v>
-      </c>
-      <c r="N20" s="1">
-        <v>82</v>
-      </c>
       <c r="O20" s="1">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
@@ -1459,16 +1459,16 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1020</v>
+        <v>120</v>
       </c>
       <c r="B21" s="1">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -1477,31 +1477,31 @@
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H21" s="1">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I21" s="1">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J21" s="1">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="K21" s="1">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21" s="1">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="N21" s="1">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="O21" s="1">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
@@ -1509,16 +1509,16 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1021</v>
+        <v>121</v>
       </c>
       <c r="B22" s="1">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -1527,31 +1527,31 @@
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="H22" s="1">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="I22" s="1">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J22" s="1">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="K22" s="1">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="L22" s="1">
         <v>0</v>
       </c>
       <c r="M22" s="1">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="N22" s="1">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="O22" s="1">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="P22" s="1">
         <v>0</v>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1022</v>
+        <v>122</v>
       </c>
       <c r="B23" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -1577,31 +1577,31 @@
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="H23" s="1">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="I23" s="1">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J23" s="1">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="K23" s="1">
+        <v>99</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
         <v>95</v>
       </c>
-      <c r="L23" s="1">
-        <v>0</v>
-      </c>
-      <c r="M23" s="1">
-        <v>98</v>
-      </c>
       <c r="N23" s="1">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="O23" s="1">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
@@ -1609,16 +1609,16 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1023</v>
+        <v>123</v>
       </c>
       <c r="B24" s="1">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
       </c>
       <c r="D24" s="1">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -1627,25 +1627,25 @@
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="H24" s="1">
         <v>70</v>
       </c>
       <c r="I24" s="1">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="J24" s="1">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="K24" s="1">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="L24" s="1">
         <v>0</v>
       </c>
       <c r="M24" s="1">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N24" s="1">
         <v>87</v>
@@ -1659,16 +1659,16 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1024</v>
+        <v>124</v>
       </c>
       <c r="B25" s="1">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
       </c>
       <c r="D25" s="1">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -1677,31 +1677,31 @@
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="H25" s="1">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="I25" s="1">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="J25" s="1">
         <v>91</v>
       </c>
       <c r="K25" s="1">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="L25" s="1">
         <v>0</v>
       </c>
       <c r="M25" s="1">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="N25" s="1">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="O25" s="1">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="P25" s="1">
         <v>0</v>
@@ -1709,16 +1709,16 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1025</v>
+        <v>125</v>
       </c>
       <c r="B26" s="1">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
       </c>
       <c r="D26" s="1">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -1727,31 +1727,31 @@
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H26" s="1">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I26" s="1">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J26" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K26" s="1">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L26" s="1">
         <v>0</v>
       </c>
       <c r="M26" s="1">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="N26" s="1">
         <v>89</v>
       </c>
       <c r="O26" s="1">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="P26" s="1">
         <v>0</v>
@@ -1759,49 +1759,49 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1026</v>
+        <v>126</v>
       </c>
       <c r="B27" s="1">
+        <v>67</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>60</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>81</v>
+      </c>
+      <c r="H27" s="1">
+        <v>94</v>
+      </c>
+      <c r="I27" s="1">
+        <v>84</v>
+      </c>
+      <c r="J27" s="1">
+        <v>57</v>
+      </c>
+      <c r="K27" s="1">
+        <v>82</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
         <v>79</v>
       </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1">
-        <v>95</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
-        <v>0</v>
-      </c>
-      <c r="G27" s="1">
-        <v>61</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="N27" s="1">
+        <v>70</v>
+      </c>
+      <c r="O27" s="1">
         <v>97</v>
-      </c>
-      <c r="I27" s="1">
-        <v>57</v>
-      </c>
-      <c r="J27" s="1">
-        <v>79</v>
-      </c>
-      <c r="K27" s="1">
-        <v>92</v>
-      </c>
-      <c r="L27" s="1">
-        <v>0</v>
-      </c>
-      <c r="M27" s="1">
-        <v>100</v>
-      </c>
-      <c r="N27" s="1">
-        <v>89</v>
-      </c>
-      <c r="O27" s="1">
-        <v>96</v>
       </c>
       <c r="P27" s="1">
         <v>0</v>
@@ -1809,16 +1809,16 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1027</v>
+        <v>127</v>
       </c>
       <c r="B28" s="1">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
       </c>
       <c r="D28" s="1">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -1827,28 +1827,28 @@
         <v>0</v>
       </c>
       <c r="G28" s="1">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H28" s="1">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="I28" s="1">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J28" s="1">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="K28" s="1">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="L28" s="1">
         <v>0</v>
       </c>
       <c r="M28" s="1">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="N28" s="1">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="O28" s="1">
         <v>98</v>
@@ -1859,16 +1859,16 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>1028</v>
+        <v>128</v>
       </c>
       <c r="B29" s="1">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
       </c>
       <c r="D29" s="1">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -1877,31 +1877,31 @@
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H29" s="1">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I29" s="1">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="J29" s="1">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="K29" s="1">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="L29" s="1">
         <v>0</v>
       </c>
       <c r="M29" s="1">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="N29" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O29" s="1">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="P29" s="1">
         <v>0</v>
@@ -1909,49 +1909,49 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>1029</v>
+        <v>129</v>
       </c>
       <c r="B30" s="1">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
       </c>
       <c r="D30" s="1">
+        <v>91</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>89</v>
+      </c>
+      <c r="H30" s="1">
+        <v>91</v>
+      </c>
+      <c r="I30" s="1">
         <v>88</v>
       </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
+      <c r="J30" s="1">
+        <v>73</v>
+      </c>
+      <c r="K30" s="1">
+        <v>88</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>82</v>
+      </c>
+      <c r="N30" s="1">
         <v>68</v>
       </c>
-      <c r="H30" s="1">
-        <v>67</v>
-      </c>
-      <c r="I30" s="1">
-        <v>69</v>
-      </c>
-      <c r="J30" s="1">
-        <v>91</v>
-      </c>
-      <c r="K30" s="1">
-        <v>66</v>
-      </c>
-      <c r="L30" s="1">
-        <v>0</v>
-      </c>
-      <c r="M30" s="1">
-        <v>84</v>
-      </c>
-      <c r="N30" s="1">
+      <c r="O30" s="1">
         <v>92</v>
-      </c>
-      <c r="O30" s="1">
-        <v>76</v>
       </c>
       <c r="P30" s="1">
         <v>0</v>
@@ -1959,16 +1959,16 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1030</v>
+        <v>130</v>
       </c>
       <c r="B31" s="1">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
       </c>
       <c r="D31" s="1">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -1977,31 +1977,31 @@
         <v>0</v>
       </c>
       <c r="G31" s="1">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="H31" s="1">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="I31" s="1">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="J31" s="1">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="K31" s="1">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L31" s="1">
         <v>0</v>
       </c>
       <c r="M31" s="1">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="N31" s="1">
         <v>83</v>
       </c>
       <c r="O31" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P31" s="1">
         <v>0</v>
@@ -2009,16 +2009,16 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1031</v>
+        <v>131</v>
       </c>
       <c r="B32" s="1">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
       </c>
       <c r="D32" s="1">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -2027,31 +2027,31 @@
         <v>0</v>
       </c>
       <c r="G32" s="1">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H32" s="1">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I32" s="1">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="J32" s="1">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="K32" s="1">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L32" s="1">
         <v>0</v>
       </c>
       <c r="M32" s="1">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="N32" s="1">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="O32" s="1">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="P32" s="1">
         <v>0</v>
@@ -2059,16 +2059,16 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1032</v>
+        <v>132</v>
       </c>
       <c r="B33" s="1">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
       </c>
       <c r="D33" s="1">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -2077,31 +2077,31 @@
         <v>0</v>
       </c>
       <c r="G33" s="1">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="H33" s="1">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="I33" s="1">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="J33" s="1">
+        <v>86</v>
+      </c>
+      <c r="K33" s="1">
+        <v>87</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
         <v>82</v>
       </c>
-      <c r="K33" s="1">
-        <v>74</v>
-      </c>
-      <c r="L33" s="1">
-        <v>0</v>
-      </c>
-      <c r="M33" s="1">
-        <v>92</v>
-      </c>
       <c r="N33" s="1">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="O33" s="1">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="P33" s="1">
         <v>0</v>
@@ -2109,16 +2109,16 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>1033</v>
+        <v>133</v>
       </c>
       <c r="B34" s="1">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" s="1">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
@@ -2127,31 +2127,31 @@
         <v>0</v>
       </c>
       <c r="G34" s="1">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="H34" s="1">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="I34" s="1">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J34" s="1">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K34" s="1">
+        <v>84</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>96</v>
+      </c>
+      <c r="N34" s="1">
         <v>80</v>
       </c>
-      <c r="L34" s="1">
-        <v>0</v>
-      </c>
-      <c r="M34" s="1">
-        <v>85</v>
-      </c>
-      <c r="N34" s="1">
-        <v>92</v>
-      </c>
       <c r="O34" s="1">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="P34" s="1">
         <v>0</v>
@@ -2159,16 +2159,16 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>1034</v>
+        <v>134</v>
       </c>
       <c r="B35" s="1">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
       </c>
       <c r="D35" s="1">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
@@ -2177,31 +2177,31 @@
         <v>0</v>
       </c>
       <c r="G35" s="1">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="H35" s="1">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="I35" s="1">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J35" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K35" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L35" s="1">
         <v>0</v>
       </c>
       <c r="M35" s="1">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N35" s="1">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="O35" s="1">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="P35" s="1">
         <v>0</v>
@@ -2209,17 +2209,17 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1035</v>
+        <v>135</v>
       </c>
       <c r="B36" s="1">
+        <v>68</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
         <v>85</v>
       </c>
-      <c r="C36" s="1">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1">
-        <v>73</v>
-      </c>
       <c r="E36" s="1">
         <v>0</v>
       </c>
@@ -2227,31 +2227,31 @@
         <v>0</v>
       </c>
       <c r="G36" s="1">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H36" s="1">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="I36" s="1">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J36" s="1">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K36" s="1">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L36" s="1">
         <v>0</v>
       </c>
       <c r="M36" s="1">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="N36" s="1">
+        <v>83</v>
+      </c>
+      <c r="O36" s="1">
         <v>94</v>
-      </c>
-      <c r="O36" s="1">
-        <v>74</v>
       </c>
       <c r="P36" s="1">
         <v>0</v>
@@ -2259,16 +2259,16 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>1036</v>
+        <v>136</v>
       </c>
       <c r="B37" s="1">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
       </c>
       <c r="D37" s="1">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -2277,31 +2277,31 @@
         <v>0</v>
       </c>
       <c r="G37" s="1">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H37" s="1">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="I37" s="1">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J37" s="1">
+        <v>63</v>
+      </c>
+      <c r="K37" s="1">
         <v>84</v>
       </c>
-      <c r="K37" s="1">
-        <v>95</v>
-      </c>
       <c r="L37" s="1">
         <v>0</v>
       </c>
       <c r="M37" s="1">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="N37" s="1">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="O37" s="1">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="P37" s="1">
         <v>0</v>

</xml_diff>